<commit_message>
feat: add new code for product
</commit_message>
<xml_diff>
--- a/result/glucose_acetate_for_yli.xlsx
+++ b/result/glucose_acetate_for_yli.xlsx
@@ -466,10 +466,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3170749310576198</v>
+        <v>0.3170749310565528</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01761527394764555</v>
+        <v>0.01761527394758626</v>
       </c>
     </row>
     <row r="3">
@@ -483,10 +483,10 @@
         <v>-0.3103448275862069</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3165994529835874</v>
+        <v>0.3165994529825238</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01758885849908819</v>
+        <v>0.0175888584990291</v>
       </c>
     </row>
     <row r="4">
@@ -500,10 +500,10 @@
         <v>-0.6206896551724137</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3155566601931394</v>
+        <v>0.3155566601920721</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01753092556628552</v>
+        <v>0.01753092556622622</v>
       </c>
     </row>
     <row r="5">
@@ -517,10 +517,10 @@
         <v>-0.9310344827586206</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3140263962681084</v>
+        <v>0.3140263962670482</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0174459109037838</v>
+        <v>0.0174459109037249</v>
       </c>
     </row>
     <row r="6">
@@ -534,10 +534,10 @@
         <v>-1.241379310344827</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3124652123231724</v>
+        <v>0.3124652123221129</v>
       </c>
       <c r="E6" t="n">
-        <v>0.01735917846239847</v>
+        <v>0.0173591784623396</v>
       </c>
     </row>
     <row r="7">
@@ -551,10 +551,10 @@
         <v>-1.551724137931034</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3106063140299954</v>
+        <v>0.3106063140289422</v>
       </c>
       <c r="E7" t="n">
-        <v>0.01725590633499975</v>
+        <v>0.01725590633494124</v>
       </c>
     </row>
     <row r="8">
@@ -568,10 +568,10 @@
         <v>-1.862068965517241</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3087474157368184</v>
+        <v>0.3087474157357716</v>
       </c>
       <c r="E8" t="n">
-        <v>0.01715263420760102</v>
+        <v>0.01715263420754286</v>
       </c>
     </row>
     <row r="9">
@@ -585,10 +585,10 @@
         <v>-2.172413793103448</v>
       </c>
       <c r="D9" t="n">
-        <v>0.3068885174436413</v>
+        <v>0.3068885174426009</v>
       </c>
       <c r="E9" t="n">
-        <v>0.01704936208020229</v>
+        <v>0.01704936208014449</v>
       </c>
     </row>
     <row r="10">
@@ -602,10 +602,10 @@
         <v>-2.482758620689655</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3049153244853561</v>
+        <v>0.304915324484314</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01693974024918645</v>
+        <v>0.01693974024912855</v>
       </c>
     </row>
     <row r="11">
@@ -619,10 +619,10 @@
         <v>-2.793103448275862</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3023271854500171</v>
+        <v>0.3023271854489665</v>
       </c>
       <c r="E11" t="n">
-        <v>0.01679595474722317</v>
+        <v>0.01679595474716481</v>
       </c>
     </row>
     <row r="12">
@@ -636,10 +636,10 @@
         <v>-3.103448275862069</v>
       </c>
       <c r="D12" t="n">
-        <v>0.299501031677348</v>
+        <v>0.2995010316763073</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01663894620429711</v>
+        <v>0.01663894620423929</v>
       </c>
     </row>
     <row r="13">
@@ -653,10 +653,10 @@
         <v>-3.413793103448276</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2966748779046789</v>
+        <v>0.296674877903648</v>
       </c>
       <c r="E13" t="n">
-        <v>0.01648193766137105</v>
+        <v>0.01648193766131378</v>
       </c>
     </row>
     <row r="14">
@@ -670,10 +670,10 @@
         <v>-3.724137931034483</v>
       </c>
       <c r="D14" t="n">
-        <v>0.293824321477752</v>
+        <v>0.2938243214767211</v>
       </c>
       <c r="E14" t="n">
-        <v>0.01632357341543067</v>
+        <v>0.01632357341537339</v>
       </c>
     </row>
     <row r="15">
@@ -687,10 +687,10 @@
         <v>-4.03448275862069</v>
       </c>
       <c r="D15" t="n">
-        <v>0.290929199043686</v>
+        <v>0.2909291990426645</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01616273328020478</v>
+        <v>0.01616273328014803</v>
       </c>
     </row>
     <row r="16">
@@ -704,10 +704,10 @@
         <v>-4.344827586206897</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2880330415823031</v>
+        <v>0.2880330415812649</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01600183564346129</v>
+        <v>0.01600183564340361</v>
       </c>
     </row>
     <row r="17">
@@ -721,10 +721,10 @@
         <v>-4.655172413793103</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2849549762495009</v>
+        <v>0.2849549762484738</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01583083201386117</v>
+        <v>0.0158308320138041</v>
       </c>
     </row>
     <row r="18">
@@ -738,10 +738,10 @@
         <v>-4.96551724137931</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2817200748625782</v>
+        <v>0.2817200748615726</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01565111527014323</v>
+        <v>0.01565111527008737</v>
       </c>
     </row>
     <row r="19">
@@ -755,10 +755,10 @@
         <v>-5.275862068965517</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2784634431385929</v>
+        <v>0.2784634431375984</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01547019128547739</v>
+        <v>0.01547019128542213</v>
       </c>
     </row>
     <row r="20">
@@ -772,10 +772,10 @@
         <v>-5.586206896551724</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2752068114146071</v>
+        <v>0.2752068114136241</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0152892673008115</v>
+        <v>0.01528926730075689</v>
       </c>
     </row>
     <row r="21">
@@ -789,10 +789,10 @@
         <v>-5.896551724137931</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2719501796906211</v>
+        <v>0.2719501796896498</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01510834331614562</v>
+        <v>0.01510834331609166</v>
       </c>
     </row>
     <row r="22">
@@ -806,10 +806,10 @@
         <v>-6.206896551724139</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2686935479666347</v>
+        <v>0.2686935479656755</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01492741933147971</v>
+        <v>0.01492741933142641</v>
       </c>
     </row>
     <row r="23">
@@ -823,10 +823,10 @@
         <v>-6.517241379310345</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2654369162426488</v>
+        <v>0.2654369162417012</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01474649534681382</v>
+        <v>0.01474649534676118</v>
       </c>
     </row>
     <row r="24">
@@ -840,10 +840,10 @@
         <v>-6.827586206896552</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2621802845186632</v>
+        <v>0.2621802845177269</v>
       </c>
       <c r="E24" t="n">
-        <v>0.01456557136214795</v>
+        <v>0.01456557136209594</v>
       </c>
     </row>
     <row r="25">
@@ -857,10 +857,10 @@
         <v>-7.137931034482759</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2589236527946769</v>
+        <v>0.2589236527937526</v>
       </c>
       <c r="E25" t="n">
-        <v>0.01438464737748205</v>
+        <v>0.0143846473774307</v>
       </c>
     </row>
     <row r="26">
@@ -874,10 +874,10 @@
         <v>-7.448275862068966</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2556670210706911</v>
+        <v>0.2556670210697783</v>
       </c>
       <c r="E26" t="n">
-        <v>0.01420372339281617</v>
+        <v>0.01420372339276546</v>
       </c>
     </row>
     <row r="27">
@@ -891,10 +891,10 @@
         <v>-7.758620689655173</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2524103893467038</v>
+        <v>0.252410389345804</v>
       </c>
       <c r="E27" t="n">
-        <v>0.01402279940815021</v>
+        <v>0.01402279940810022</v>
       </c>
     </row>
     <row r="28">
@@ -908,10 +908,10 @@
         <v>-8.068965517241379</v>
       </c>
       <c r="D28" t="n">
-        <v>0.24893593705541</v>
+        <v>0.2489359370545267</v>
       </c>
       <c r="E28" t="n">
-        <v>0.01382977428085611</v>
+        <v>0.01382977428080704</v>
       </c>
     </row>
     <row r="29">
@@ -925,10 +925,10 @@
         <v>-8.379310344827587</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2453807609982925</v>
+        <v>0.2453807609974218</v>
       </c>
       <c r="E29" t="n">
-        <v>0.01363226449990514</v>
+        <v>0.01363226449985677</v>
       </c>
     </row>
     <row r="30">
@@ -942,10 +942,10 @@
         <v>-8.689655172413794</v>
       </c>
       <c r="D30" t="n">
-        <v>0.2418255849411763</v>
+        <v>0.2418255849403169</v>
       </c>
       <c r="E30" t="n">
-        <v>0.01343475471895424</v>
+        <v>0.01343475471890649</v>
       </c>
     </row>
     <row r="31">
@@ -959,10 +959,10 @@
         <v>-9</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2382704088840575</v>
+        <v>0.238270408883212</v>
       </c>
       <c r="E31" t="n">
-        <v>0.01323724493800319</v>
+        <v>0.01323724493795622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>